<commit_message>
SQL query generator first commit
</commit_message>
<xml_diff>
--- a/transformation_files/Transformation_logic.xlsx
+++ b/transformation_files/Transformation_logic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sambe\Desktop\ETL_GENAI_project\transformation_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5BFBD3-9572-456C-A4BA-8CACE63E4C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35728B0-3D98-4601-BCE0-5E696EE052F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{AC3B4EE2-A014-412A-8B8A-0ECDDCB5FF02}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
   <si>
     <t>source_table</t>
   </si>
@@ -129,6 +129,42 @@
   </si>
   <si>
     <t>concat "OO5" before order id</t>
+  </si>
+  <si>
+    <t>cust_id</t>
+  </si>
+  <si>
+    <t>product_id</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>case when effdate&lt;'2023-10-01' then "old" else new</t>
+  </si>
+  <si>
+    <t>effdate</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>item_effdate</t>
+  </si>
+  <si>
+    <t>item_code</t>
+  </si>
+  <si>
+    <t>discounted_price</t>
+  </si>
+  <si>
+    <t>item_discount_price</t>
+  </si>
+  <si>
+    <t>discount price by 15%</t>
   </si>
 </sst>
 </file>
@@ -494,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79CDB5C-740B-4D9E-AB6A-9FAC3356CB62}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -615,7 +651,7 @@
         <v>16</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>17</v>
@@ -692,48 +728,159 @@
         <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" ht="103.25" x14ac:dyDescent="0.75">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>